<commit_message>
Update after delete geo-not-NYC
</commit_message>
<xml_diff>
--- a/Project4 final_project/weekday_and_hour_speed.xlsx
+++ b/Project4 final_project/weekday_and_hour_speed.xlsx
@@ -16,6 +16,19 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>上到下為一到日</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>左到右為0時到23時</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,8 +619,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -795,6 +811,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$1:$X$1</c:f>
@@ -802,76 +899,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>16.599889100736</c:v>
+                  <c:v>16.536475397343001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.2645421839924</c:v>
+                  <c:v>17.216074497802801</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.3212429643085</c:v>
+                  <c:v>17.259428304576101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.106586446115202</c:v>
+                  <c:v>17.982410766272601</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.504519361509001</c:v>
+                  <c:v>21.204415247246299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.211631099566201</c:v>
+                  <c:v>20.9727427754563</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.642015819013301</c:v>
+                  <c:v>15.5657792734699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.420294162101801</c:v>
+                  <c:v>11.3665645706714</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0064106835840594</c:v>
+                  <c:v>8.9531674914420005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6591534400289003</c:v>
+                  <c:v>8.6108264759343598</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.7119198077058897</c:v>
+                  <c:v>8.6233425562939203</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.6824707287930103</c:v>
+                  <c:v>8.5922235998253296</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.8574031502027797</c:v>
+                  <c:v>8.7792237896444796</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.0780683587572604</c:v>
+                  <c:v>8.9702034227180096</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.1426747073036001</c:v>
+                  <c:v>9.0059926472888101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.99564528243239</c:v>
+                  <c:v>8.9052554235387902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.5211664506063105</c:v>
+                  <c:v>9.4519856502628308</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.2822154560682595</c:v>
+                  <c:v>9.2394954061150099</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.4119977154640893</c:v>
+                  <c:v>9.3801695635968407</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.8003782223009</c:v>
+                  <c:v>10.7636678625698</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.1041432444758</c:v>
+                  <c:v>12.0583637833076</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.453191308080299</c:v>
+                  <c:v>12.4055483427287</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.924111505019299</c:v>
+                  <c:v>12.8606916583211</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.333829730868899</c:v>
+                  <c:v>14.306778382251499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -896,6 +993,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$2:$X$2</c:f>
@@ -903,76 +1081,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>18.064568193222499</c:v>
+                  <c:v>18.003306793097099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.734808397045999</c:v>
+                  <c:v>19.625201717742499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.8681982286124</c:v>
+                  <c:v>20.9123737193888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.8385640942499</c:v>
+                  <c:v>22.555546870438199</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.1572537416688</c:v>
+                  <c:v>22.850649667369598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.423786732640099</c:v>
+                  <c:v>19.759574956946899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.3125628679675</c:v>
+                  <c:v>16.179838655922001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.7427995473018</c:v>
+                  <c:v>11.703933322669201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3418694398272795</c:v>
+                  <c:v>9.3033837491001599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6922435904730406</c:v>
+                  <c:v>8.6481880599071292</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.9916314362787002</c:v>
+                  <c:v>8.9453621156843894</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.6855787935111906</c:v>
+                  <c:v>8.5951025490628492</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0732217477381205</c:v>
+                  <c:v>8.9952942891515093</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.0561206685962006</c:v>
+                  <c:v>8.9710677966896508</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.9061845286269392</c:v>
+                  <c:v>8.8123559070408692</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.6488420841858993</c:v>
+                  <c:v>8.5589204707286708</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1329355133336207</c:v>
+                  <c:v>9.0902709133020103</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.7863561535791703</c:v>
+                  <c:v>8.7744071650635806</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.8711078299239006</c:v>
+                  <c:v>8.8131754844701007</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.633357080249199</c:v>
+                  <c:v>10.6018902648528</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.196860285768899</c:v>
+                  <c:v>12.168133395315801</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.8650855156978</c:v>
+                  <c:v>12.815695366102499</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.3132434653951</c:v>
+                  <c:v>13.2601669699366</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15.222993895797</c:v>
+                  <c:v>15.1160273573404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,6 +1175,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$3:$X$3</c:f>
@@ -1004,76 +1263,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>20.6667065568605</c:v>
+                  <c:v>20.553589355183799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.502628714960601</c:v>
+                  <c:v>22.412571676188499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.638464145446498</c:v>
+                  <c:v>23.545970154151501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.623163976422699</c:v>
+                  <c:v>27.246880466498101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.496524542424499</c:v>
+                  <c:v>24.9985134321267</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.973812533443301</c:v>
+                  <c:v>21.269579283772501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.899398258417801</c:v>
+                  <c:v>16.710679606241801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.8656489788334</c:v>
+                  <c:v>11.729619683391199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2345357734436995</c:v>
+                  <c:v>9.1796862316860803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7559912098805608</c:v>
+                  <c:v>8.6762618661629691</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.2067529894720792</c:v>
+                  <c:v>9.1694864013450008</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.8935324008953494</c:v>
+                  <c:v>8.7721320026011291</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.2741096180381906</c:v>
+                  <c:v>9.1928115081462707</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.4899834511556005</c:v>
+                  <c:v>9.3633164069848895</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.3457859425720997</c:v>
+                  <c:v>9.2178711131717694</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.0668126421668394</c:v>
+                  <c:v>8.9589350338884408</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.09297808713489</c:v>
+                  <c:v>9.0362577446241996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.7092490336260209</c:v>
+                  <c:v>8.6665852318725705</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.1473528035108291</c:v>
+                  <c:v>9.0974594334337393</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.807260543901601</c:v>
+                  <c:v>10.797598330938801</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.0427009646061</c:v>
+                  <c:v>11.9907474475963</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.926528020286</c:v>
+                  <c:v>12.8762454093764</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.5932119788067</c:v>
+                  <c:v>13.5051761702032</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17.281448621613301</c:v>
+                  <c:v>17.167982638671901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,6 +1357,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$4:$X$4</c:f>
@@ -1105,76 +1445,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>26.378300045625</c:v>
+                  <c:v>26.327807315853399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.045621553573902</c:v>
+                  <c:v>32.849329705933798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.287425635113003</c:v>
+                  <c:v>39.0996288355243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.384211238683903</c:v>
+                  <c:v>47.1076880240308</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.991474282015197</c:v>
+                  <c:v>38.226203033800303</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.800675530356301</c:v>
+                  <c:v>24.0981154518267</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.7350536610401</c:v>
+                  <c:v>15.5335396655531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.437419698970601</c:v>
+                  <c:v>11.3018391687855</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.35856527654812</c:v>
+                  <c:v>9.3067818486863594</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6922453742409598</c:v>
+                  <c:v>8.6431389334462807</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.2735843437065704</c:v>
+                  <c:v>9.2019164446886208</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.1343364314823798</c:v>
+                  <c:v>9.0166882499419891</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.86114780413698</c:v>
+                  <c:v>9.7692858071639002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.2750929065833</c:v>
+                  <c:v>10.1944007057714</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.9764354526030097</c:v>
+                  <c:v>9.8503722094611597</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.2462587973804204</c:v>
+                  <c:v>9.1877481178724008</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.4298728169205397</c:v>
+                  <c:v>9.4139821848100507</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.5068645978804103</c:v>
+                  <c:v>9.4620761054731304</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.47944585842599</c:v>
+                  <c:v>9.4340239535024697</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.810611447389499</c:v>
+                  <c:v>10.770165718835001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.2045577866858</c:v>
+                  <c:v>11.163522353171601</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.1991021691922</c:v>
+                  <c:v>11.1833463670607</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.8661788973996</c:v>
+                  <c:v>12.8495482083448</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17.431459690594199</c:v>
+                  <c:v>17.355271652635899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,6 +1539,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$5:$X$5</c:f>
@@ -1206,76 +1627,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>31.232139337197101</c:v>
+                  <c:v>31.099618583193401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.630477187469303</c:v>
+                  <c:v>49.443789296117501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.623887173715303</c:v>
+                  <c:v>73.295661094126402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.643413189906596</c:v>
+                  <c:v>86.5444189946449</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.419795042068898</c:v>
+                  <c:v>54.9907221911756</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.708955906447699</c:v>
+                  <c:v>19.4026113046829</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0738454607097108</c:v>
+                  <c:v>8.8816560400122597</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4542826382888903</c:v>
+                  <c:v>6.3587357262019397</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0417070212384596</c:v>
+                  <c:v>6.9790160262133796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.4625285633734695</c:v>
+                  <c:v>9.3799460896745295</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.0691054188443</c:v>
+                  <c:v>12.038411744839699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.8161017793408</c:v>
+                  <c:v>11.7615736257249</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.3756186938255</c:v>
+                  <c:v>12.2865121579697</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.070372748454499</c:v>
+                  <c:v>12.013431969973899</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.8933750938534</c:v>
+                  <c:v>10.8526145448369</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.215050197218</c:v>
+                  <c:v>11.124505523506601</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.6254321752004</c:v>
+                  <c:v>11.5755093783701</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.4272812404476</c:v>
+                  <c:v>10.3756966696336</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.3703664345720501</c:v>
+                  <c:v>9.3361241322884094</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.5320318724477797</c:v>
+                  <c:v>9.5232958773093799</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.1314430765600001</c:v>
+                  <c:v>9.1249450892830808</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.6660142570804801</c:v>
+                  <c:v>9.6636323185155497</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.516906262397001</c:v>
+                  <c:v>11.5007995258915</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>16.892298653845799</c:v>
+                  <c:v>16.8746690430646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1300,6 +1721,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$6:$X$6</c:f>
@@ -1307,76 +1809,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>32.138094639932099</c:v>
+                  <c:v>32.123818464308002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.867152530872097</c:v>
+                  <c:v>52.737076689493101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.164137073473597</c:v>
+                  <c:v>76.119325850268197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.413087179162403</c:v>
+                  <c:v>97.0564736007709</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62.815508943672697</c:v>
+                  <c:v>62.766995074353801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.969537447525699</c:v>
+                  <c:v>18.561905550845001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2806006575214006</c:v>
+                  <c:v>8.1507335079836807</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6943212722508196</c:v>
+                  <c:v>5.5608406679857998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2964780335271504</c:v>
+                  <c:v>6.2218342692584496</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7434442766754703</c:v>
+                  <c:v>8.6273947549391092</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.6440142629804</c:v>
+                  <c:v>12.527470959060199</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.984214066551299</c:v>
+                  <c:v>12.878343437403901</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.9151274792258</c:v>
+                  <c:v>12.8473056725857</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.531413622961599</c:v>
+                  <c:v>12.419829663456699</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.6645151973081</c:v>
+                  <c:v>11.5280143000724</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.6160933756858</c:v>
+                  <c:v>11.4750999981484</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.664713044535301</c:v>
+                  <c:v>12.566006415112501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.230196693615699</c:v>
+                  <c:v>11.1470061199689</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.4252865792713898</c:v>
+                  <c:v>9.3728817345657092</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.3773054409418393</c:v>
+                  <c:v>9.3541394874442894</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.4181428496957906</c:v>
+                  <c:v>9.3925931773751898</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.6700036670915299</c:v>
+                  <c:v>9.6396395150698897</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.3902068148415</c:v>
+                  <c:v>10.369954854649601</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.2099061180612</c:v>
+                  <c:v>12.128490000317001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1403,6 +1905,87 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weekday_and_hour_speed2!$A$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20833333333333301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70833333333333304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79166666666666696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833333333333304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>weekday_and_hour_speed2!$A$7:$X$7</c:f>
@@ -1410,76 +1993,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>17.300675428895801</c:v>
+                  <c:v>17.2261930719032</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.906028713234701</c:v>
+                  <c:v>17.823602466529099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.1007583065239</c:v>
+                  <c:v>19.004089433508899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.141026244890099</c:v>
+                  <c:v>21.770627287251902</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.595183483159801</c:v>
+                  <c:v>26.130125979601999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.365364429584599</c:v>
+                  <c:v>21.934704610255899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.5996786520653</c:v>
+                  <c:v>15.4673505044358</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.729843876259</c:v>
+                  <c:v>10.665910441893301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.1080079466238804</c:v>
+                  <c:v>9.0474417778697802</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0452572909065196</c:v>
+                  <c:v>8.9777121851562391</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3056221680971394</c:v>
+                  <c:v>9.2330977774645895</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.3269075335629505</c:v>
+                  <c:v>9.2487182712018399</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.5561612512304901</c:v>
+                  <c:v>9.4331821052090792</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.8636555710450207</c:v>
+                  <c:v>9.7746058606861705</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.9152178448153894</c:v>
+                  <c:v>9.8342801568045495</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.2344305713395</c:v>
+                  <c:v>10.105018797616699</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.835261818773899</c:v>
+                  <c:v>10.800300078728499</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.091003841077001</c:v>
+                  <c:v>10.0530601256621</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.0394265088003</c:v>
+                  <c:v>9.9961902090076293</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.0024228935049</c:v>
+                  <c:v>10.962163508853701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.794686784321099</c:v>
+                  <c:v>11.763413603288299</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.924829810123899</c:v>
+                  <c:v>11.8655454386061</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.6453543372445</c:v>
+                  <c:v>11.601099637916599</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.5481114405173</c:v>
+                  <c:v>12.5049213545391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,11 +2078,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="229458688"/>
-        <c:axId val="740605920"/>
+        <c:axId val="208693392"/>
+        <c:axId val="208693952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="229458688"/>
+        <c:axId val="208693392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,7 +2145,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1599,7 +2182,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="740605920"/>
+        <c:crossAx val="208693952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1607,7 +2190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="740605920"/>
+        <c:axId val="208693952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +2298,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229458688"/>
+        <c:crossAx val="208693392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2359,13 +2942,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>219076</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2650,530 +3233,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>16.599889100736</v>
+        <v>16.536475397343001</v>
       </c>
       <c r="B1">
-        <v>17.2645421839924</v>
+        <v>17.216074497802801</v>
       </c>
       <c r="C1">
-        <v>17.3212429643085</v>
+        <v>17.259428304576101</v>
       </c>
       <c r="D1">
-        <v>18.106586446115202</v>
+        <v>17.982410766272601</v>
       </c>
       <c r="E1">
-        <v>21.504519361509001</v>
+        <v>21.204415247246299</v>
       </c>
       <c r="F1">
-        <v>21.211631099566201</v>
+        <v>20.9727427754563</v>
       </c>
       <c r="G1">
-        <v>15.642015819013301</v>
+        <v>15.5657792734699</v>
       </c>
       <c r="H1">
-        <v>11.420294162101801</v>
+        <v>11.3665645706714</v>
       </c>
       <c r="I1">
-        <v>9.0064106835840594</v>
+        <v>8.9531674914420005</v>
       </c>
       <c r="J1">
-        <v>8.6591534400289003</v>
+        <v>8.6108264759343598</v>
       </c>
       <c r="K1">
-        <v>8.7119198077058897</v>
+        <v>8.6233425562939203</v>
       </c>
       <c r="L1">
-        <v>8.6824707287930103</v>
+        <v>8.5922235998253296</v>
       </c>
       <c r="M1">
-        <v>8.8574031502027797</v>
+        <v>8.7792237896444796</v>
       </c>
       <c r="N1">
-        <v>9.0780683587572604</v>
+        <v>8.9702034227180096</v>
       </c>
       <c r="O1">
-        <v>9.1426747073036001</v>
+        <v>9.0059926472888101</v>
       </c>
       <c r="P1">
-        <v>8.99564528243239</v>
+        <v>8.9052554235387902</v>
       </c>
       <c r="Q1">
-        <v>9.5211664506063105</v>
+        <v>9.4519856502628308</v>
       </c>
       <c r="R1">
-        <v>9.2822154560682595</v>
+        <v>9.2394954061150099</v>
       </c>
       <c r="S1">
-        <v>9.4119977154640893</v>
+        <v>9.3801695635968407</v>
       </c>
       <c r="T1">
-        <v>10.8003782223009</v>
+        <v>10.7636678625698</v>
       </c>
       <c r="U1">
-        <v>12.1041432444758</v>
+        <v>12.0583637833076</v>
       </c>
       <c r="V1">
-        <v>12.453191308080299</v>
+        <v>12.4055483427287</v>
       </c>
       <c r="W1">
-        <v>12.924111505019299</v>
+        <v>12.8606916583211</v>
       </c>
       <c r="X1">
-        <v>14.333829730868899</v>
+        <v>14.306778382251499</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18.064568193222499</v>
+        <v>18.003306793097099</v>
       </c>
       <c r="B2">
-        <v>19.734808397045999</v>
+        <v>19.625201717742499</v>
       </c>
       <c r="C2">
-        <v>20.8681982286124</v>
+        <v>20.9123737193888</v>
       </c>
       <c r="D2">
-        <v>22.8385640942499</v>
+        <v>22.555546870438199</v>
       </c>
       <c r="E2">
-        <v>23.1572537416688</v>
+        <v>22.850649667369598</v>
       </c>
       <c r="F2">
-        <v>20.423786732640099</v>
+        <v>19.759574956946899</v>
       </c>
       <c r="G2">
-        <v>16.3125628679675</v>
+        <v>16.179838655922001</v>
       </c>
       <c r="H2">
-        <v>11.7427995473018</v>
+        <v>11.703933322669201</v>
       </c>
       <c r="I2">
-        <v>9.3418694398272795</v>
+        <v>9.3033837491001599</v>
       </c>
       <c r="J2">
-        <v>8.6922435904730406</v>
+        <v>8.6481880599071292</v>
       </c>
       <c r="K2">
-        <v>8.9916314362787002</v>
+        <v>8.9453621156843894</v>
       </c>
       <c r="L2">
-        <v>8.6855787935111906</v>
+        <v>8.5951025490628492</v>
       </c>
       <c r="M2">
-        <v>9.0732217477381205</v>
+        <v>8.9952942891515093</v>
       </c>
       <c r="N2">
-        <v>9.0561206685962006</v>
+        <v>8.9710677966896508</v>
       </c>
       <c r="O2">
-        <v>8.9061845286269392</v>
+        <v>8.8123559070408692</v>
       </c>
       <c r="P2">
-        <v>8.6488420841858993</v>
+        <v>8.5589204707286708</v>
       </c>
       <c r="Q2">
-        <v>9.1329355133336207</v>
+        <v>9.0902709133020103</v>
       </c>
       <c r="R2">
-        <v>8.7863561535791703</v>
+        <v>8.7744071650635806</v>
       </c>
       <c r="S2">
-        <v>8.8711078299239006</v>
+        <v>8.8131754844701007</v>
       </c>
       <c r="T2">
-        <v>10.633357080249199</v>
+        <v>10.6018902648528</v>
       </c>
       <c r="U2">
-        <v>12.196860285768899</v>
+        <v>12.168133395315801</v>
       </c>
       <c r="V2">
-        <v>12.8650855156978</v>
+        <v>12.815695366102499</v>
       </c>
       <c r="W2">
-        <v>13.3132434653951</v>
+        <v>13.2601669699366</v>
       </c>
       <c r="X2">
-        <v>15.222993895797</v>
+        <v>15.1160273573404</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20.6667065568605</v>
+        <v>20.553589355183799</v>
       </c>
       <c r="B3">
-        <v>22.502628714960601</v>
+        <v>22.412571676188499</v>
       </c>
       <c r="C3">
-        <v>23.638464145446498</v>
+        <v>23.545970154151501</v>
       </c>
       <c r="D3">
-        <v>27.623163976422699</v>
+        <v>27.246880466498101</v>
       </c>
       <c r="E3">
-        <v>25.496524542424499</v>
+        <v>24.9985134321267</v>
       </c>
       <c r="F3">
-        <v>21.973812533443301</v>
+        <v>21.269579283772501</v>
       </c>
       <c r="G3">
-        <v>16.899398258417801</v>
+        <v>16.710679606241801</v>
       </c>
       <c r="H3">
-        <v>11.8656489788334</v>
+        <v>11.729619683391199</v>
       </c>
       <c r="I3">
-        <v>9.2345357734436995</v>
+        <v>9.1796862316860803</v>
       </c>
       <c r="J3">
-        <v>8.7559912098805608</v>
+        <v>8.6762618661629691</v>
       </c>
       <c r="K3">
-        <v>9.2067529894720792</v>
+        <v>9.1694864013450008</v>
       </c>
       <c r="L3">
-        <v>8.8935324008953494</v>
+        <v>8.7721320026011291</v>
       </c>
       <c r="M3">
-        <v>9.2741096180381906</v>
+        <v>9.1928115081462707</v>
       </c>
       <c r="N3">
-        <v>9.4899834511556005</v>
+        <v>9.3633164069848895</v>
       </c>
       <c r="O3">
-        <v>9.3457859425720997</v>
+        <v>9.2178711131717694</v>
       </c>
       <c r="P3">
-        <v>9.0668126421668394</v>
+        <v>8.9589350338884408</v>
       </c>
       <c r="Q3">
-        <v>9.09297808713489</v>
+        <v>9.0362577446241996</v>
       </c>
       <c r="R3">
-        <v>8.7092490336260209</v>
+        <v>8.6665852318725705</v>
       </c>
       <c r="S3">
-        <v>9.1473528035108291</v>
+        <v>9.0974594334337393</v>
       </c>
       <c r="T3">
-        <v>10.807260543901601</v>
+        <v>10.797598330938801</v>
       </c>
       <c r="U3">
-        <v>12.0427009646061</v>
+        <v>11.9907474475963</v>
       </c>
       <c r="V3">
-        <v>12.926528020286</v>
+        <v>12.8762454093764</v>
       </c>
       <c r="W3">
-        <v>13.5932119788067</v>
+        <v>13.5051761702032</v>
       </c>
       <c r="X3">
-        <v>17.281448621613301</v>
+        <v>17.167982638671901</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>26.378300045625</v>
+        <v>26.327807315853399</v>
       </c>
       <c r="B4">
-        <v>33.045621553573902</v>
+        <v>32.849329705933798</v>
       </c>
       <c r="C4">
-        <v>39.287425635113003</v>
+        <v>39.0996288355243</v>
       </c>
       <c r="D4">
-        <v>47.384211238683903</v>
+        <v>47.1076880240308</v>
       </c>
       <c r="E4">
-        <v>38.991474282015197</v>
+        <v>38.226203033800303</v>
       </c>
       <c r="F4">
-        <v>24.800675530356301</v>
+        <v>24.0981154518267</v>
       </c>
       <c r="G4">
-        <v>15.7350536610401</v>
+        <v>15.5335396655531</v>
       </c>
       <c r="H4">
-        <v>11.437419698970601</v>
+        <v>11.3018391687855</v>
       </c>
       <c r="I4">
-        <v>9.35856527654812</v>
+        <v>9.3067818486863594</v>
       </c>
       <c r="J4">
-        <v>8.6922453742409598</v>
+        <v>8.6431389334462807</v>
       </c>
       <c r="K4">
-        <v>9.2735843437065704</v>
+        <v>9.2019164446886208</v>
       </c>
       <c r="L4">
-        <v>9.1343364314823798</v>
+        <v>9.0166882499419891</v>
       </c>
       <c r="M4">
-        <v>9.86114780413698</v>
+        <v>9.7692858071639002</v>
       </c>
       <c r="N4">
-        <v>10.2750929065833</v>
+        <v>10.1944007057714</v>
       </c>
       <c r="O4">
-        <v>9.9764354526030097</v>
+        <v>9.8503722094611597</v>
       </c>
       <c r="P4">
-        <v>9.2462587973804204</v>
+        <v>9.1877481178724008</v>
       </c>
       <c r="Q4">
-        <v>9.4298728169205397</v>
+        <v>9.4139821848100507</v>
       </c>
       <c r="R4">
-        <v>9.5068645978804103</v>
+        <v>9.4620761054731304</v>
       </c>
       <c r="S4">
-        <v>9.47944585842599</v>
+        <v>9.4340239535024697</v>
       </c>
       <c r="T4">
-        <v>10.810611447389499</v>
+        <v>10.770165718835001</v>
       </c>
       <c r="U4">
-        <v>11.2045577866858</v>
+        <v>11.163522353171601</v>
       </c>
       <c r="V4">
-        <v>11.1991021691922</v>
+        <v>11.1833463670607</v>
       </c>
       <c r="W4">
-        <v>12.8661788973996</v>
+        <v>12.8495482083448</v>
       </c>
       <c r="X4">
-        <v>17.431459690594199</v>
+        <v>17.355271652635899</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>31.232139337197101</v>
+        <v>31.099618583193401</v>
       </c>
       <c r="B5">
-        <v>49.630477187469303</v>
+        <v>49.443789296117501</v>
       </c>
       <c r="C5">
-        <v>73.623887173715303</v>
+        <v>73.295661094126402</v>
       </c>
       <c r="D5">
-        <v>86.643413189906596</v>
+        <v>86.5444189946449</v>
       </c>
       <c r="E5">
-        <v>55.419795042068898</v>
+        <v>54.9907221911756</v>
       </c>
       <c r="F5">
-        <v>19.708955906447699</v>
+        <v>19.4026113046829</v>
       </c>
       <c r="G5">
-        <v>9.0738454607097108</v>
+        <v>8.8816560400122597</v>
       </c>
       <c r="H5">
-        <v>6.4542826382888903</v>
+        <v>6.3587357262019397</v>
       </c>
       <c r="I5">
-        <v>7.0417070212384596</v>
+        <v>6.9790160262133796</v>
       </c>
       <c r="J5">
-        <v>9.4625285633734695</v>
+        <v>9.3799460896745295</v>
       </c>
       <c r="K5">
-        <v>12.0691054188443</v>
+        <v>12.038411744839699</v>
       </c>
       <c r="L5">
-        <v>11.8161017793408</v>
+        <v>11.7615736257249</v>
       </c>
       <c r="M5">
-        <v>12.3756186938255</v>
+        <v>12.2865121579697</v>
       </c>
       <c r="N5">
-        <v>12.070372748454499</v>
+        <v>12.013431969973899</v>
       </c>
       <c r="O5">
-        <v>10.8933750938534</v>
+        <v>10.8526145448369</v>
       </c>
       <c r="P5">
-        <v>11.215050197218</v>
+        <v>11.124505523506601</v>
       </c>
       <c r="Q5">
-        <v>11.6254321752004</v>
+        <v>11.5755093783701</v>
       </c>
       <c r="R5">
-        <v>10.4272812404476</v>
+        <v>10.3756966696336</v>
       </c>
       <c r="S5">
-        <v>9.3703664345720501</v>
+        <v>9.3361241322884094</v>
       </c>
       <c r="T5">
-        <v>9.5320318724477797</v>
+        <v>9.5232958773093799</v>
       </c>
       <c r="U5">
-        <v>9.1314430765600001</v>
+        <v>9.1249450892830808</v>
       </c>
       <c r="V5">
-        <v>9.6660142570804801</v>
+        <v>9.6636323185155497</v>
       </c>
       <c r="W5">
-        <v>11.516906262397001</v>
+        <v>11.5007995258915</v>
       </c>
       <c r="X5">
-        <v>16.892298653845799</v>
+        <v>16.8746690430646</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>32.138094639932099</v>
+        <v>32.123818464308002</v>
       </c>
       <c r="B6">
-        <v>52.867152530872097</v>
+        <v>52.737076689493101</v>
       </c>
       <c r="C6">
-        <v>76.164137073473597</v>
+        <v>76.119325850268197</v>
       </c>
       <c r="D6">
-        <v>97.413087179162403</v>
+        <v>97.0564736007709</v>
       </c>
       <c r="E6">
-        <v>62.815508943672697</v>
+        <v>62.766995074353801</v>
       </c>
       <c r="F6">
-        <v>18.969537447525699</v>
+        <v>18.561905550845001</v>
       </c>
       <c r="G6">
-        <v>8.2806006575214006</v>
+        <v>8.1507335079836807</v>
       </c>
       <c r="H6">
-        <v>5.6943212722508196</v>
+        <v>5.5608406679857998</v>
       </c>
       <c r="I6">
-        <v>6.2964780335271504</v>
+        <v>6.2218342692584496</v>
       </c>
       <c r="J6">
-        <v>8.7434442766754703</v>
+        <v>8.6273947549391092</v>
       </c>
       <c r="K6">
-        <v>12.6440142629804</v>
+        <v>12.527470959060199</v>
       </c>
       <c r="L6">
-        <v>12.984214066551299</v>
+        <v>12.878343437403901</v>
       </c>
       <c r="M6">
-        <v>12.9151274792258</v>
+        <v>12.8473056725857</v>
       </c>
       <c r="N6">
-        <v>12.531413622961599</v>
+        <v>12.419829663456699</v>
       </c>
       <c r="O6">
-        <v>11.6645151973081</v>
+        <v>11.5280143000724</v>
       </c>
       <c r="P6">
-        <v>11.6160933756858</v>
+        <v>11.4750999981484</v>
       </c>
       <c r="Q6">
-        <v>12.664713044535301</v>
+        <v>12.566006415112501</v>
       </c>
       <c r="R6">
-        <v>11.230196693615699</v>
+        <v>11.1470061199689</v>
       </c>
       <c r="S6">
-        <v>9.4252865792713898</v>
+        <v>9.3728817345657092</v>
       </c>
       <c r="T6">
-        <v>9.3773054409418393</v>
+        <v>9.3541394874442894</v>
       </c>
       <c r="U6">
-        <v>9.4181428496957906</v>
+        <v>9.3925931773751898</v>
       </c>
       <c r="V6">
-        <v>9.6700036670915299</v>
+        <v>9.6396395150698897</v>
       </c>
       <c r="W6">
-        <v>10.3902068148415</v>
+        <v>10.369954854649601</v>
       </c>
       <c r="X6">
-        <v>12.2099061180612</v>
+        <v>12.128490000317001</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>17.300675428895801</v>
+        <v>17.2261930719032</v>
       </c>
       <c r="B7">
-        <v>17.906028713234701</v>
+        <v>17.823602466529099</v>
       </c>
       <c r="C7">
-        <v>19.1007583065239</v>
+        <v>19.004089433508899</v>
       </c>
       <c r="D7">
-        <v>22.141026244890099</v>
+        <v>21.770627287251902</v>
       </c>
       <c r="E7">
-        <v>26.595183483159801</v>
+        <v>26.130125979601999</v>
       </c>
       <c r="F7">
-        <v>22.365364429584599</v>
+        <v>21.934704610255899</v>
       </c>
       <c r="G7">
-        <v>15.5996786520653</v>
+        <v>15.4673505044358</v>
       </c>
       <c r="H7">
-        <v>10.729843876259</v>
+        <v>10.665910441893301</v>
       </c>
       <c r="I7">
-        <v>9.1080079466238804</v>
+        <v>9.0474417778697802</v>
       </c>
       <c r="J7">
-        <v>9.0452572909065196</v>
+        <v>8.9777121851562391</v>
       </c>
       <c r="K7">
-        <v>9.3056221680971394</v>
+        <v>9.2330977774645895</v>
       </c>
       <c r="L7">
-        <v>9.3269075335629505</v>
+        <v>9.2487182712018399</v>
       </c>
       <c r="M7">
-        <v>9.5561612512304901</v>
+        <v>9.4331821052090792</v>
       </c>
       <c r="N7">
-        <v>9.8636555710450207</v>
+        <v>9.7746058606861705</v>
       </c>
       <c r="O7">
-        <v>9.9152178448153894</v>
+        <v>9.8342801568045495</v>
       </c>
       <c r="P7">
-        <v>10.2344305713395</v>
+        <v>10.105018797616699</v>
       </c>
       <c r="Q7">
-        <v>10.835261818773899</v>
+        <v>10.800300078728499</v>
       </c>
       <c r="R7">
-        <v>10.091003841077001</v>
+        <v>10.0530601256621</v>
       </c>
       <c r="S7">
-        <v>10.0394265088003</v>
+        <v>9.9961902090076293</v>
       </c>
       <c r="T7">
-        <v>11.0024228935049</v>
+        <v>10.962163508853701</v>
       </c>
       <c r="U7">
-        <v>11.794686784321099</v>
+        <v>11.763413603288299</v>
       </c>
       <c r="V7">
-        <v>11.924829810123899</v>
+        <v>11.8655454386061</v>
       </c>
       <c r="W7">
-        <v>11.6453543372445</v>
+        <v>11.601099637916599</v>
       </c>
       <c r="X7">
-        <v>12.5481114405173</v>
+        <v>12.5049213545391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>